<commit_message>
cihuyy kode baru lagi kita cuy
</commit_message>
<xml_diff>
--- a/peminjaman/Daftar_Peminjaman.xlsx
+++ b/peminjaman/Daftar_Peminjaman.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>No</t>
   </si>
@@ -35,22 +35,19 @@
     <t>Status Peminjaman</t>
   </si>
   <si>
+    <t>alcoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dilan &amp; milea </t>
+  </si>
+  <si>
+    <t>2024-02-16</t>
+  </si>
+  <si>
+    <t>Dikembalikan</t>
+  </si>
+  <si>
     <t>fahrezi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dilan &amp; milea </t>
-  </si>
-  <si>
-    <t>2024-02-15</t>
-  </si>
-  <si>
-    <t>Dikembalikan</t>
-  </si>
-  <si>
-    <t>alcoy</t>
-  </si>
-  <si>
-    <t>2024-02-16</t>
   </si>
 </sst>
 </file>
@@ -449,10 +446,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -463,16 +460,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -483,16 +480,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>

</xml_diff>